<commit_message>
Final commit, other than bugtesting and fixing
</commit_message>
<xml_diff>
--- a/Sample1.xlsx
+++ b/Sample1.xlsx
@@ -3,103 +3,283 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7865E2CB-CF93-44A5-80DD-F46F858533E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE087D1-541F-4E3F-8A20-222B54F50E76}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2898" yWindow="2898" windowWidth="17280" windowHeight="8994" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test1" sheetId="1" r:id="rId1"/>
     <sheet name="Test2" sheetId="2" r:id="rId2"/>
     <sheet name="Test3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
-  <si>
-    <t>Box #</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>File Name</t>
   </si>
   <si>
-    <t>SHPD001</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 01</t>
-  </si>
-  <si>
-    <t>TEST 01</t>
-  </si>
-  <si>
-    <t>TEST 02</t>
-  </si>
-  <si>
-    <t>TEST 03</t>
-  </si>
-  <si>
-    <t>TEST 04</t>
-  </si>
-  <si>
-    <t>TEST 05</t>
-  </si>
-  <si>
-    <t>TEST 06</t>
-  </si>
-  <si>
-    <t>TEST 07</t>
-  </si>
-  <si>
-    <t>TEST 08</t>
-  </si>
-  <si>
-    <t>TEST 09</t>
-  </si>
-  <si>
-    <t>TEST 10</t>
-  </si>
-  <si>
-    <t>TEST 11</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 02</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 03</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 04</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 05</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 06</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 07</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 08</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 09</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 10</t>
-  </si>
-  <si>
-    <t>SHPD001 -- TEST 11</t>
-  </si>
-  <si>
-    <t>BARCODE</t>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>FileTest01</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest01</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest02</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest03</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest04</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest05</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest06</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest07</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest08</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest09</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest10</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest11</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest12</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest13</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest14</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest15</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest16</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest17</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest18</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest19</t>
+  </si>
+  <si>
+    <t>DD2019-BoxTest01--FileTest20</t>
+  </si>
+  <si>
+    <t>FileTest02</t>
+  </si>
+  <si>
+    <t>FileTest03</t>
+  </si>
+  <si>
+    <t>FileTest04</t>
+  </si>
+  <si>
+    <t>FileTest05</t>
+  </si>
+  <si>
+    <t>FileTest06</t>
+  </si>
+  <si>
+    <t>FileTest07</t>
+  </si>
+  <si>
+    <t>FileTest08</t>
+  </si>
+  <si>
+    <t>FileTest09</t>
+  </si>
+  <si>
+    <t>FileTest10</t>
+  </si>
+  <si>
+    <t>FileTest11</t>
+  </si>
+  <si>
+    <t>FileTest12</t>
+  </si>
+  <si>
+    <t>FileTest13</t>
+  </si>
+  <si>
+    <t>FileTest14</t>
+  </si>
+  <si>
+    <t>FileTest15</t>
+  </si>
+  <si>
+    <t>FileTest16</t>
+  </si>
+  <si>
+    <t>FileTest17</t>
+  </si>
+  <si>
+    <t>FileTest18</t>
+  </si>
+  <si>
+    <t>FileTest19</t>
+  </si>
+  <si>
+    <t>FileTest20</t>
+  </si>
+  <si>
+    <t>1BOXTEST01</t>
+  </si>
+  <si>
+    <t>1BOXTEST02</t>
+  </si>
+  <si>
+    <t>1BOXTEST03</t>
+  </si>
+  <si>
+    <t>1BOXTEST04</t>
+  </si>
+  <si>
+    <t>1BOXTEST05</t>
+  </si>
+  <si>
+    <t>1BOXTEST06</t>
+  </si>
+  <si>
+    <t>1BOXTEST07</t>
+  </si>
+  <si>
+    <t>1BOXTEST08</t>
+  </si>
+  <si>
+    <t>1BOXTEST09</t>
+  </si>
+  <si>
+    <t>1BOXTEST10</t>
+  </si>
+  <si>
+    <t>1BOXTEST11</t>
+  </si>
+  <si>
+    <t>1BOXTEST12</t>
+  </si>
+  <si>
+    <t>1BOXTEST13</t>
+  </si>
+  <si>
+    <t>1BOXTEST14</t>
+  </si>
+  <si>
+    <t>1BOXTEST15</t>
+  </si>
+  <si>
+    <t>1BOXTEST16</t>
+  </si>
+  <si>
+    <t>1BOXTEST17</t>
+  </si>
+  <si>
+    <t>1BOXTEST18</t>
+  </si>
+  <si>
+    <t>1BOXTEST19</t>
+  </si>
+  <si>
+    <t>1BOXTEST20</t>
+  </si>
+  <si>
+    <t>1BOXTEST21</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST01</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST02</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST03</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST04</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST05</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST06</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST07</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST08</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST09</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST10</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST11</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST12</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST13</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST14</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST15</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST16</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST17</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST18</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST19</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST20</t>
+  </si>
+  <si>
+    <t>DD20191FILETEST21</t>
   </si>
 </sst>
 </file>
@@ -417,171 +597,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="29.83984375" customWidth="1"/>
+    <col min="2" max="2" width="21.3671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B478CE94-B5AB-40EA-A532-3EFBFCE2C78D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60A4405-BA86-4B17-B746-3C532BB55EF1}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
+    <col min="1" max="1" width="30.68359375" customWidth="1"/>
+    <col min="2" max="2" width="25.26171875" customWidth="1"/>
     <col min="3" max="3" width="17.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
+      <c r="B21" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>